<commit_message>
test: calculate testbench run time and bus usage times
Signed-off-by: Ben Lancaster <bdl@live.co.uk>
</commit_message>
<xml_diff>
--- a/docs/reports/sum_cores.xlsx
+++ b/docs/reports/sum_cores.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\uni\vmicro16\docs\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77A86602-CCEC-4434-9D7D-AA10CFB95548}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A08F66E0-731E-4305-A1B3-C018A77FF319}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13512" windowHeight="5928" xr2:uid="{5A307FF0-66F5-4B0E-A119-9BBC50973945}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{5A307FF0-66F5-4B0E-A119-9BBC50973945}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
   <si>
     <t>Core Count</t>
   </si>
@@ -49,13 +50,48 @@
   <si>
     <t>Ideal Diff</t>
   </si>
+  <si>
+    <t>Cores</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Ncore</t>
+  </si>
+  <si>
+    <t>Ttotal</t>
+  </si>
+  <si>
+    <t>Tbus</t>
+  </si>
+  <si>
+    <t>Treq</t>
+  </si>
+  <si>
+    <t>Tfail</t>
+  </si>
+  <si>
+    <t>Tsum</t>
+  </si>
+  <si>
+    <t>Tbus_T</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -83,8 +119,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -643,6 +680,1551 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$J$48</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Tbus_T</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$J$49:$J$56</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.26</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.9379999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.62</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-2C2F-4440-869E-1FF41D3E5EB0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$I$48</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Tsum</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$I$49:$I$56</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>124.19000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>65.069999999999993</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43.851999999999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>34.39</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-2C2F-4440-869E-1FF41D3E5EB0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="221"/>
+        <c:overlap val="100"/>
+        <c:axId val="455287328"/>
+        <c:axId val="455282080"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="3"/>
+                <c:order val="2"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$F$48</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Tbus</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent4"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:dLbls>
+                  <c:spPr>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                  <c:txPr>
+                    <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                      <a:spAutoFit/>
+                    </a:bodyPr>
+                    <a:lstStyle/>
+                    <a:p>
+                      <a:pPr>
+                        <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                          <a:solidFill>
+                            <a:schemeClr val="tx1">
+                              <a:lumMod val="75000"/>
+                              <a:lumOff val="25000"/>
+                            </a:schemeClr>
+                          </a:solidFill>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:defRPr>
+                      </a:pPr>
+                      <a:endParaRPr lang="en-US"/>
+                    </a:p>
+                  </c:txPr>
+                  <c:showLegendKey val="0"/>
+                  <c:showVal val="1"/>
+                  <c:showCatName val="0"/>
+                  <c:showSerName val="0"/>
+                  <c:showPercent val="0"/>
+                  <c:showBubbleSize val="0"/>
+                  <c:showLeaderLines val="0"/>
+                  <c:extLst>
+                    <c:ext uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                      <c15:showLeaderLines val="1"/>
+                      <c15:leaderLines>
+                        <c:spPr>
+                          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1">
+                                <a:lumMod val="35000"/>
+                                <a:lumOff val="65000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                            <a:round/>
+                          </a:ln>
+                          <a:effectLst/>
+                        </c:spPr>
+                      </c15:leaderLines>
+                    </c:ext>
+                  </c:extLst>
+                </c:dLbls>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$F$49:$F$56</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="8"/>
+                      <c:pt idx="0">
+                        <c:v>16</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>31.5</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>32.299999999999997</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>57.75</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000003-2C2F-4440-869E-1FF41D3E5EB0}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredBarSeries>
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="3"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$E$48</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Ttotal</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent1"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:dLbls>
+                  <c:spPr>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                  <c:txPr>
+                    <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                      <a:spAutoFit/>
+                    </a:bodyPr>
+                    <a:lstStyle/>
+                    <a:p>
+                      <a:pPr>
+                        <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                          <a:solidFill>
+                            <a:schemeClr val="tx1">
+                              <a:lumMod val="75000"/>
+                              <a:lumOff val="25000"/>
+                            </a:schemeClr>
+                          </a:solidFill>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:defRPr>
+                      </a:pPr>
+                      <a:endParaRPr lang="en-US"/>
+                    </a:p>
+                  </c:txPr>
+                  <c:showLegendKey val="0"/>
+                  <c:showVal val="1"/>
+                  <c:showCatName val="0"/>
+                  <c:showSerName val="0"/>
+                  <c:showPercent val="0"/>
+                  <c:showBubbleSize val="0"/>
+                  <c:showLeaderLines val="0"/>
+                  <c:extLst>
+                    <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                      <c15:showLeaderLines val="1"/>
+                      <c15:leaderLines>
+                        <c:spPr>
+                          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1">
+                                <a:lumMod val="35000"/>
+                                <a:lumOff val="65000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                            <a:round/>
+                          </a:ln>
+                          <a:effectLst/>
+                        </c:spPr>
+                      </c15:leaderLines>
+                    </c:ext>
+                  </c:extLst>
+                </c:dLbls>
+                <c:cat>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$B$49:$B$56</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="8"/>
+                      <c:pt idx="0">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>8</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>16</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>32</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>64</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$E$49:$E$56</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="8"/>
+                      <c:pt idx="0">
+                        <c:v>124.51</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>66.33</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>45.79</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>39.01</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000000-2C2F-4440-869E-1FF41D3E5EB0}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredBarSeries>
+          </c:ext>
+        </c:extLst>
+      </c:barChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="455287328"/>
+        <c:axId val="455282080"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="2"/>
+                <c:order val="4"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$G$48</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Treq</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent3"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:dLbls>
+                  <c:spPr>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                  <c:txPr>
+                    <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                      <a:spAutoFit/>
+                    </a:bodyPr>
+                    <a:lstStyle/>
+                    <a:p>
+                      <a:pPr>
+                        <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                          <a:solidFill>
+                            <a:schemeClr val="tx1">
+                              <a:lumMod val="75000"/>
+                              <a:lumOff val="25000"/>
+                            </a:schemeClr>
+                          </a:solidFill>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:defRPr>
+                      </a:pPr>
+                      <a:endParaRPr lang="en-US"/>
+                    </a:p>
+                  </c:txPr>
+                  <c:showLegendKey val="0"/>
+                  <c:showVal val="1"/>
+                  <c:showCatName val="0"/>
+                  <c:showSerName val="0"/>
+                  <c:showPercent val="0"/>
+                  <c:showBubbleSize val="0"/>
+                  <c:showLeaderLines val="0"/>
+                  <c:extLst>
+                    <c:ext uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                      <c15:showLeaderLines val="1"/>
+                      <c15:leaderLines>
+                        <c:spPr>
+                          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1">
+                                <a:lumMod val="35000"/>
+                                <a:lumOff val="65000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                            <a:round/>
+                          </a:ln>
+                          <a:effectLst/>
+                        </c:spPr>
+                      </c15:leaderLines>
+                    </c:ext>
+                  </c:extLst>
+                </c:dLbls>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$G$49:$G$56</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="8"/>
+                      <c:pt idx="0">
+                        <c:v>8</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>10.5</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>9</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>13.25</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000002-2C2F-4440-869E-1FF41D3E5EB0}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+          </c:ext>
+        </c:extLst>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="455287328"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="455282080"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="455282080"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="455287328"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -676,6 +2258,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>184537</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>183544</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>489337</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>183544</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C13264A4-C002-416F-A4E0-1B61A2BDC0D7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -981,10 +2599,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B42E696D-D336-41B5-94F4-79A874490BCA}">
-  <dimension ref="A1:F43"/>
+  <dimension ref="A1:J56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J52" sqref="J52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -993,6 +2611,8 @@
     <col min="2" max="2" width="10.77734375" customWidth="1"/>
     <col min="3" max="3" width="11.5546875" customWidth="1"/>
     <col min="4" max="4" width="11.77734375" customWidth="1"/>
+    <col min="5" max="5" width="9.77734375" customWidth="1"/>
+    <col min="10" max="10" width="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -1027,7 +2647,7 @@
         <v>125</v>
       </c>
       <c r="E2">
-        <f t="shared" ref="E2:E10" si="0">(B13/B2)</f>
+        <f>(B13/B2)</f>
         <v>125</v>
       </c>
       <c r="F2">
@@ -1043,18 +2663,18 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C10" si="1">(A3/B3)</f>
+        <f t="shared" ref="C3:C10" si="0">(A3/B3)</f>
         <v>120</v>
       </c>
       <c r="D3">
         <v>66</v>
       </c>
       <c r="E3">
-        <f t="shared" si="0"/>
+        <f>(B14/B3)</f>
         <v>62.5</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F10" si="2">(D3-E3)</f>
+        <f>(D3-E3)</f>
         <v>3.5</v>
       </c>
     </row>
@@ -1066,18 +2686,18 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>80</v>
       </c>
       <c r="D4">
         <v>47.05</v>
       </c>
       <c r="E4">
-        <f t="shared" si="0"/>
+        <f>(B15/B4)</f>
         <v>41.666666666666664</v>
       </c>
       <c r="F4">
-        <f t="shared" si="2"/>
+        <f>(D4-E4)</f>
         <v>5.3833333333333329</v>
       </c>
     </row>
@@ -1089,18 +2709,18 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>60</v>
       </c>
       <c r="D5">
         <v>40</v>
       </c>
       <c r="E5">
-        <f t="shared" si="0"/>
+        <f>(B16/B5)</f>
         <v>31.25</v>
       </c>
       <c r="F5">
-        <f t="shared" si="2"/>
+        <f>(D5-E5)</f>
         <v>8.75</v>
       </c>
     </row>
@@ -1112,18 +2732,18 @@
         <v>8</v>
       </c>
       <c r="C6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="D6">
         <v>30</v>
       </c>
       <c r="E6">
-        <f t="shared" si="0"/>
+        <f>(B17/B6)</f>
         <v>15.625</v>
       </c>
       <c r="F6">
-        <f t="shared" si="2"/>
+        <f>(D6-E6)</f>
         <v>14.375</v>
       </c>
     </row>
@@ -1135,15 +2755,15 @@
         <v>12</v>
       </c>
       <c r="C7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="E7">
-        <f t="shared" si="0"/>
+        <f>(B18/B7)</f>
         <v>10.416666666666666</v>
       </c>
       <c r="F7">
-        <f t="shared" si="2"/>
+        <f>(D7-E7)</f>
         <v>-10.416666666666666</v>
       </c>
     </row>
@@ -1155,15 +2775,15 @@
         <v>16</v>
       </c>
       <c r="C8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="E8">
-        <f t="shared" si="0"/>
+        <f>(B19/B8)</f>
         <v>7.8125</v>
       </c>
       <c r="F8">
-        <f t="shared" si="2"/>
+        <f>(D8-E8)</f>
         <v>-7.8125</v>
       </c>
     </row>
@@ -1175,15 +2795,15 @@
         <v>32</v>
       </c>
       <c r="C9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>7.5</v>
       </c>
       <c r="E9">
-        <f t="shared" si="0"/>
+        <f>(B20/B9)</f>
         <v>3.90625</v>
       </c>
       <c r="F9">
-        <f t="shared" si="2"/>
+        <f>(D9-E9)</f>
         <v>-3.90625</v>
       </c>
     </row>
@@ -1195,15 +2815,15 @@
         <v>64</v>
       </c>
       <c r="C10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3.75</v>
       </c>
       <c r="E10">
-        <f t="shared" si="0"/>
+        <f>(B21/B10)</f>
         <v>1.953125</v>
       </c>
       <c r="F10">
-        <f t="shared" si="2"/>
+        <f>(D10-E10)</f>
         <v>-1.953125</v>
       </c>
     </row>
@@ -1285,7 +2905,7 @@
         <v>240</v>
       </c>
       <c r="E24">
-        <f t="shared" ref="E24:E32" si="3">(B35/B24)</f>
+        <f>(B35/B24)</f>
         <v>0</v>
       </c>
       <c r="F24">
@@ -1301,18 +2921,18 @@
         <v>2</v>
       </c>
       <c r="C25">
-        <f t="shared" ref="C25:C32" si="4">(A25/B25)</f>
+        <f t="shared" ref="C25:C32" si="1">(A25/B25)</f>
         <v>120</v>
       </c>
       <c r="D25">
         <v>66.13</v>
       </c>
       <c r="E25">
-        <f t="shared" si="3"/>
+        <f>(B36/B25)</f>
         <v>62.5</v>
       </c>
       <c r="F25">
-        <f t="shared" ref="F25:F32" si="5">(D25-E25)</f>
+        <f>(D25-E25)</f>
         <v>3.6299999999999955</v>
       </c>
     </row>
@@ -1324,15 +2944,15 @@
         <v>3</v>
       </c>
       <c r="C26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>80</v>
       </c>
       <c r="E26">
-        <f t="shared" si="3"/>
+        <f>(B37/B26)</f>
         <v>41.666666666666664</v>
       </c>
       <c r="F26">
-        <f t="shared" si="5"/>
+        <f>(D26-E26)</f>
         <v>-41.666666666666664</v>
       </c>
     </row>
@@ -1344,18 +2964,18 @@
         <v>4</v>
       </c>
       <c r="C27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>60</v>
       </c>
       <c r="D27">
         <v>38.090000000000003</v>
       </c>
       <c r="E27">
-        <f t="shared" si="3"/>
+        <f>(B38/B27)</f>
         <v>31.25</v>
       </c>
       <c r="F27">
-        <f t="shared" si="5"/>
+        <f>(D27-E27)</f>
         <v>6.8400000000000034</v>
       </c>
     </row>
@@ -1367,18 +2987,18 @@
         <v>8</v>
       </c>
       <c r="C28">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="D28">
         <v>35.29</v>
       </c>
       <c r="E28">
-        <f t="shared" si="3"/>
+        <f>(B39/B28)</f>
         <v>15.625</v>
       </c>
       <c r="F28">
-        <f t="shared" si="5"/>
+        <f>(D28-E28)</f>
         <v>19.664999999999999</v>
       </c>
     </row>
@@ -1390,18 +3010,18 @@
         <v>12</v>
       </c>
       <c r="C29">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="D29">
         <v>45</v>
       </c>
       <c r="E29">
-        <f t="shared" si="3"/>
+        <f>(B40/B29)</f>
         <v>10.416666666666666</v>
       </c>
       <c r="F29">
-        <f t="shared" si="5"/>
+        <f>(D29-E29)</f>
         <v>34.583333333333336</v>
       </c>
     </row>
@@ -1413,18 +3033,18 @@
         <v>16</v>
       </c>
       <c r="C30">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="D30">
         <v>65.75</v>
       </c>
       <c r="E30">
-        <f t="shared" si="3"/>
+        <f>(B41/B30)</f>
         <v>7.8125</v>
       </c>
       <c r="F30">
-        <f t="shared" si="5"/>
+        <f>(D30-E30)</f>
         <v>57.9375</v>
       </c>
     </row>
@@ -1436,15 +3056,15 @@
         <v>32</v>
       </c>
       <c r="C31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>7.5</v>
       </c>
       <c r="E31">
-        <f t="shared" si="3"/>
+        <f>(B42/B31)</f>
         <v>3.90625</v>
       </c>
       <c r="F31">
-        <f t="shared" si="5"/>
+        <f>(D31-E31)</f>
         <v>-3.90625</v>
       </c>
     </row>
@@ -1456,19 +3076,19 @@
         <v>64</v>
       </c>
       <c r="C32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>3.75</v>
       </c>
       <c r="E32">
-        <f t="shared" si="3"/>
+        <f>(B43/B32)</f>
         <v>1.953125</v>
       </c>
       <c r="F32">
-        <f t="shared" si="5"/>
+        <f>(D32-E32)</f>
         <v>-1.953125</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>4</v>
       </c>
@@ -1477,48 +3097,274 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B36">
         <v>125</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B37">
         <v>125</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B38">
         <v>125</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B39">
         <v>125</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B40">
         <v>125</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B41">
         <v>125</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B42">
         <v>125</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B43">
         <v>125</v>
       </c>
     </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>7</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C48" t="s">
+        <v>8</v>
+      </c>
+      <c r="E48" t="s">
+        <v>9</v>
+      </c>
+      <c r="F48" t="s">
+        <v>10</v>
+      </c>
+      <c r="G48" t="s">
+        <v>11</v>
+      </c>
+      <c r="H48" t="s">
+        <v>12</v>
+      </c>
+      <c r="I48" t="s">
+        <v>13</v>
+      </c>
+      <c r="J48" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>240</v>
+      </c>
+      <c r="B49" s="1">
+        <v>1</v>
+      </c>
+      <c r="C49">
+        <f>(A49/B49)</f>
+        <v>240</v>
+      </c>
+      <c r="E49">
+        <v>124.51</v>
+      </c>
+      <c r="F49">
+        <v>16</v>
+      </c>
+      <c r="G49">
+        <v>8</v>
+      </c>
+      <c r="I49">
+        <f>(E49-J49)</f>
+        <v>124.19000000000001</v>
+      </c>
+      <c r="J49">
+        <f>(F49*B49)*(20*POWER(10, -3))</f>
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>240</v>
+      </c>
+      <c r="B50" s="1">
+        <v>2</v>
+      </c>
+      <c r="C50">
+        <f t="shared" ref="C50:C56" si="2">(A50/B50)</f>
+        <v>120</v>
+      </c>
+      <c r="E50">
+        <v>66.33</v>
+      </c>
+      <c r="F50">
+        <v>31.5</v>
+      </c>
+      <c r="G50">
+        <v>10.5</v>
+      </c>
+      <c r="I50">
+        <f t="shared" ref="I50:I56" si="3">(E50-J50)</f>
+        <v>65.069999999999993</v>
+      </c>
+      <c r="J50">
+        <f t="shared" ref="J50:J56" si="4">(F50*B50)*(20*POWER(10, -3))</f>
+        <v>1.26</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>240</v>
+      </c>
+      <c r="B51" s="1">
+        <v>3</v>
+      </c>
+      <c r="C51">
+        <f t="shared" si="2"/>
+        <v>80</v>
+      </c>
+      <c r="E51">
+        <v>45.79</v>
+      </c>
+      <c r="F51">
+        <v>32.299999999999997</v>
+      </c>
+      <c r="G51">
+        <v>9</v>
+      </c>
+      <c r="I51">
+        <f t="shared" si="3"/>
+        <v>43.851999999999997</v>
+      </c>
+      <c r="J51">
+        <f t="shared" si="4"/>
+        <v>1.9379999999999999</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>240</v>
+      </c>
+      <c r="B52" s="1">
+        <v>4</v>
+      </c>
+      <c r="C52">
+        <f t="shared" si="2"/>
+        <v>60</v>
+      </c>
+      <c r="E52">
+        <v>39.01</v>
+      </c>
+      <c r="F52">
+        <v>57.75</v>
+      </c>
+      <c r="G52">
+        <v>13.25</v>
+      </c>
+      <c r="I52">
+        <f t="shared" si="3"/>
+        <v>34.39</v>
+      </c>
+      <c r="J52">
+        <f t="shared" si="4"/>
+        <v>4.62</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>240</v>
+      </c>
+      <c r="B53" s="1">
+        <v>8</v>
+      </c>
+      <c r="C53">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="I53">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J53">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>240</v>
+      </c>
+      <c r="B54" s="1">
+        <v>16</v>
+      </c>
+      <c r="C54">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="I54">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J54">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>240</v>
+      </c>
+      <c r="B55" s="1">
+        <v>32</v>
+      </c>
+      <c r="C55">
+        <f t="shared" si="2"/>
+        <v>7.5</v>
+      </c>
+      <c r="I55">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J55">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>240</v>
+      </c>
+      <c r="B56" s="1">
+        <v>64</v>
+      </c>
+      <c r="C56">
+        <f t="shared" si="2"/>
+        <v>3.75</v>
+      </c>
+      <c r="I56">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J56">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
report: sum_cores.xlsx for instruction fetching
Signed-off-by: Ben Lancaster <bdl@live.co.uk>
</commit_message>
<xml_diff>
--- a/docs/reports/sum_cores.xlsx
+++ b/docs/reports/sum_cores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\uni\vmicro16\docs\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A797D7B9-64CB-4F5D-9865-31729E875E25}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDB6A722-DB42-4E4F-B5E7-05E3E68D8BE1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{5A307FF0-66F5-4B0E-A119-9BBC50973945}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="16">
   <si>
     <t>Core Count</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>Tbus_T</t>
+  </si>
+  <si>
+    <t>Tinstr_T</t>
   </si>
 </sst>
 </file>
@@ -1846,6 +1849,807 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Algorithm</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> Time vs Core Count (N = 240)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$J$72</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Tbus_T</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$49:$B$56</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>30</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$J$73:$J$80</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="4">
+                  <c:v>24</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0350-4141-B3C0-FBB53C3B5536}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$I$72</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Tsum</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$49:$B$56</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>30</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$I$73:$I$80</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-13.269999999999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0350-4141-B3C0-FBB53C3B5536}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$K$72</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Tinstr_T</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$K$73:$K$80</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="4">
+                  <c:v>87.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-0350-4141-B3C0-FBB53C3B5536}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="ctr"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="221"/>
+        <c:overlap val="100"/>
+        <c:axId val="455287328"/>
+        <c:axId val="455282080"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="455287328"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Core Count</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="455282080"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="455282080"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Total</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Time (us)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="455287328"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1926,6 +2730,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -2430,6 +3274,509 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3037,6 +4384,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>457199</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>134470</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>161364</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>134470</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{10E4EA5E-C4C9-4232-87F6-1D0956074AD9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3342,10 +4727,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B42E696D-D336-41B5-94F4-79A874490BCA}">
-  <dimension ref="A1:J57"/>
+  <dimension ref="A1:K80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="P64" sqref="P64"/>
+    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K79" sqref="K79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4140,6 +5525,181 @@
     <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B57" s="1"/>
     </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>7</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C72" t="s">
+        <v>8</v>
+      </c>
+      <c r="E72" t="s">
+        <v>9</v>
+      </c>
+      <c r="F72" t="s">
+        <v>10</v>
+      </c>
+      <c r="G72" t="s">
+        <v>11</v>
+      </c>
+      <c r="H72" t="s">
+        <v>12</v>
+      </c>
+      <c r="I72" t="s">
+        <v>13</v>
+      </c>
+      <c r="J72" t="s">
+        <v>14</v>
+      </c>
+      <c r="K72" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A73">
+        <v>240</v>
+      </c>
+      <c r="B73" s="1">
+        <v>1</v>
+      </c>
+      <c r="C73">
+        <f>(A73/B73)</f>
+        <v>240</v>
+      </c>
+      <c r="I73">
+        <f>(E73-J73)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A74">
+        <v>240</v>
+      </c>
+      <c r="B74" s="1">
+        <v>2</v>
+      </c>
+      <c r="C74">
+        <f t="shared" ref="C74:C80" si="9">(A74/B74)</f>
+        <v>120</v>
+      </c>
+      <c r="I74">
+        <f t="shared" ref="I74:I80" si="10">(E74-J74)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <v>240</v>
+      </c>
+      <c r="B75" s="1">
+        <v>3</v>
+      </c>
+      <c r="C75">
+        <f t="shared" si="9"/>
+        <v>80</v>
+      </c>
+      <c r="I75">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A76">
+        <v>240</v>
+      </c>
+      <c r="B76" s="1">
+        <v>4</v>
+      </c>
+      <c r="C76">
+        <f t="shared" si="9"/>
+        <v>60</v>
+      </c>
+      <c r="I76">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A77">
+        <v>240</v>
+      </c>
+      <c r="B77" s="1">
+        <v>8</v>
+      </c>
+      <c r="C77">
+        <f t="shared" si="9"/>
+        <v>30</v>
+      </c>
+      <c r="E77">
+        <v>122.23</v>
+      </c>
+      <c r="F77">
+        <v>105</v>
+      </c>
+      <c r="G77">
+        <v>24</v>
+      </c>
+      <c r="I77">
+        <f>(E77-(J77+K77+G77))</f>
+        <v>-13.269999999999996</v>
+      </c>
+      <c r="J77">
+        <v>24</v>
+      </c>
+      <c r="K77">
+        <v>87.5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A78">
+        <v>240</v>
+      </c>
+      <c r="B78" s="1">
+        <v>12</v>
+      </c>
+      <c r="C78">
+        <f t="shared" si="9"/>
+        <v>20</v>
+      </c>
+      <c r="I78">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A79">
+        <v>240</v>
+      </c>
+      <c r="B79" s="1">
+        <v>16</v>
+      </c>
+      <c r="C79">
+        <f t="shared" si="9"/>
+        <v>15</v>
+      </c>
+      <c r="I79">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A80">
+        <v>240</v>
+      </c>
+      <c r="B80" s="1">
+        <v>30</v>
+      </c>
+      <c r="C80">
+        <f t="shared" si="9"/>
+        <v>8</v>
+      </c>
+      <c r="I80">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>